<commit_message>
Added more test files for testing all instructors functionality
</commit_message>
<xml_diff>
--- a/Example/Distribution Files/F1997/MEC E 260 - 502 (77588) Ayranci/MecE260_UNDERGRAD Grade Dist Form.xlsx
+++ b/Example/Distribution Files/F1997/MEC E 260 - 502 (77588) Ayranci/MecE260_UNDERGRAD Grade Dist Form.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\AC-UG 2021-2024\00_Grade_Approvals\Processing_Folders\Example\F2021\MEC E 260 - 502 (77588) Ayranci\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\Processing_Folders\Example\Distribution Files\F1997\MEC E 260 - 502 (77588) Ayranci\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B7D2BB-7D2B-4556-A957-BC4B63C345C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="120" windowWidth="15180" windowHeight="8835" tabRatio="475" activeTab="2"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -27,17 +28,29 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'SECOND YEAR'!$A$1:$P$55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'THIRD YEAR'!$A$1:$P$55</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. C. Sit</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -147,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -191,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -237,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -259,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -281,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -303,7 +316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -330,12 +343,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. C. Sit</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -357,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -379,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -401,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -423,7 +436,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -445,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -467,7 +480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -489,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -512,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -535,7 +548,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -557,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -579,7 +592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -601,7 +614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -628,12 +641,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. C. Sit</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -655,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -677,7 +690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -699,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -721,7 +734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -743,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -765,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -787,7 +800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -810,7 +823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -833,7 +846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -855,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -877,7 +890,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -899,7 +912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -926,12 +939,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. C. Sit</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -953,7 +966,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -975,7 +988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -997,7 +1010,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1019,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1041,7 +1054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1063,7 +1076,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1085,7 +1098,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1108,7 +1121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1131,7 +1144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1153,7 +1166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1197,7 +1210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K21" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1518,7 +1531,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1900,6 +1913,21 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1938,18 +1966,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1961,9 +1977,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2773,10 +2786,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.125</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.9375</c:v>
+                  <c:v>14.0625</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>14.0625</c:v>
@@ -2785,7 +2798,7 @@
                   <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.625</c:v>
+                  <c:v>1.5625</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14.0625</c:v>
@@ -2797,7 +2810,7 @@
                   <c:v>4.6875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2806,7 +2819,7 @@
                   <c:v>1.5625</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.8125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4230,7 +4243,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10241" name="Chart 1"/>
+        <xdr:cNvPr id="10241" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001280000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4267,7 +4286,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9217" name="Chart 1"/>
+        <xdr:cNvPr id="9217" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001240000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4304,7 +4329,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7169" name="Chart 1"/>
+        <xdr:cNvPr id="7169" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000011C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4341,7 +4372,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8193" name="Chart 1"/>
+        <xdr:cNvPr id="8193" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001200000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4708,7 +4745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -4716,29 +4753,29 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4752,7 +4789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet10">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4762,82 +4799,82 @@
       <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.703125" customWidth="1"/>
+    <col min="2" max="2" width="3.703125" customWidth="1"/>
+    <col min="3" max="4" width="8.703125" customWidth="1"/>
+    <col min="5" max="5" width="7.703125" customWidth="1"/>
+    <col min="6" max="6" width="1.703125" customWidth="1"/>
+    <col min="7" max="7" width="7.703125" customWidth="1"/>
+    <col min="8" max="8" width="1.703125" customWidth="1"/>
+    <col min="9" max="9" width="7.703125" customWidth="1"/>
+    <col min="10" max="10" width="1.703125" customWidth="1"/>
+    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.703125" customWidth="1"/>
+    <col min="13" max="13" width="1.703125" customWidth="1"/>
+    <col min="14" max="14" width="3.703125" customWidth="1"/>
+    <col min="15" max="15" width="9.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="59"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -4846,59 +4883,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="60" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="60" t="s">
+      <c r="H6" s="50"/>
+      <c r="I6" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="61"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="61"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="50"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62" t="s">
+      <c r="H7" s="52"/>
+      <c r="I7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="62" t="s">
+      <c r="L7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="63"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="52"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -4928,7 +4965,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -4959,7 +4996,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -4989,7 +5026,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -5020,7 +5057,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -5051,7 +5088,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -5082,7 +5119,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -5112,7 +5149,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -5142,7 +5179,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -5172,7 +5209,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -5202,7 +5239,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -5232,7 +5269,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -5262,11 +5299,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="65" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="66"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>0</v>
@@ -5292,24 +5329,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="67" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B22" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
+      <c r="C22" s="69"/>
+      <c r="D22" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="60" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -5319,34 +5356,34 @@
         <v>#VALUE!</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="57" t="s">
+      <c r="N22" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="58" t="e">
+      <c r="O22" s="63" t="e">
         <f>$L$22/MAX($L$23,1)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="64" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="56"/>
+      <c r="I23" s="61"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="59"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="N23" s="61"/>
+      <c r="O23" s="64"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -5364,7 +5401,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -5380,14 +5417,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -5404,7 +5441,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D28" s="20" t="s">
         <v>58</v>
       </c>
@@ -5422,6 +5459,10 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G6:H6"/>
@@ -5438,14 +5479,10 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>depts</formula1>
     </dataValidation>
   </dataValidations>
@@ -5459,96 +5496,96 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.703125" customWidth="1"/>
+    <col min="2" max="2" width="3.703125" customWidth="1"/>
+    <col min="3" max="4" width="8.703125" customWidth="1"/>
+    <col min="5" max="5" width="7.703125" customWidth="1"/>
+    <col min="6" max="6" width="1.703125" customWidth="1"/>
+    <col min="7" max="7" width="7.703125" customWidth="1"/>
+    <col min="8" max="8" width="1.703125" customWidth="1"/>
+    <col min="9" max="9" width="7.703125" customWidth="1"/>
+    <col min="10" max="10" width="1.703125" customWidth="1"/>
+    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.703125" customWidth="1"/>
+    <col min="13" max="13" width="1.703125" customWidth="1"/>
+    <col min="14" max="14" width="3.703125" customWidth="1"/>
+    <col min="15" max="15" width="9.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="50" t="s">
+      <c r="L3" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="59"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -5557,59 +5594,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="60" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="60" t="s">
+      <c r="H6" s="50"/>
+      <c r="I6" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="61"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="61"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="50"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62" t="s">
+      <c r="H7" s="52"/>
+      <c r="I7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="62" t="s">
+      <c r="L7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="63"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="52"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -5617,29 +5654,29 @@
         <v>4</v>
       </c>
       <c r="E8" s="38">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="11">
         <f t="shared" ref="G8:G19" si="0">D8*E8</f>
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="42">
         <f t="shared" ref="I8:I19" si="1">E8/MAX($E$20,1)*100</f>
-        <v>3.125</v>
+        <v>25</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7">
         <f>SUM(I$8:I8)</f>
-        <v>3.125</v>
+        <v>25</v>
       </c>
       <c r="L8" s="45">
         <v>5</v>
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -5647,22 +5684,22 @@
         <v>4</v>
       </c>
       <c r="E9" s="39">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="11">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="42">
         <f t="shared" si="1"/>
-        <v>10.9375</v>
+        <v>14.0625</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7">
         <f>SUM(I$8:I9)</f>
-        <v>14.0625</v>
+        <v>39.0625</v>
       </c>
       <c r="L9" s="46">
         <v>7</v>
@@ -5670,7 +5707,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -5693,14 +5730,14 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7">
         <f>SUM(I$8:I10)</f>
-        <v>28.125</v>
+        <v>53.125</v>
       </c>
       <c r="L10" s="45">
         <v>12</v>
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -5723,7 +5760,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7">
         <f>SUM(I$8:I11)</f>
-        <v>43.75</v>
+        <v>68.75</v>
       </c>
       <c r="L11" s="46">
         <v>15</v>
@@ -5731,7 +5768,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -5739,22 +5776,22 @@
         <v>3</v>
       </c>
       <c r="E12" s="38">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="11">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="42">
         <f t="shared" si="1"/>
-        <v>15.625</v>
+        <v>1.5625</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7">
         <f>SUM(I$8:I12)</f>
-        <v>59.375</v>
+        <v>70.3125</v>
       </c>
       <c r="L12" s="45">
         <v>16</v>
@@ -5762,7 +5799,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -5785,7 +5822,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7">
         <f>SUM(I$8:I13)</f>
-        <v>73.4375</v>
+        <v>84.375</v>
       </c>
       <c r="L13" s="46">
         <v>14</v>
@@ -5793,7 +5830,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -5816,14 +5853,14 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7">
         <f>SUM(I$8:I14)</f>
-        <v>82.8125</v>
+        <v>93.75</v>
       </c>
       <c r="L14" s="45">
         <v>11</v>
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -5846,14 +5883,14 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7">
         <f>SUM(I$8:I15)</f>
-        <v>87.5</v>
+        <v>98.4375</v>
       </c>
       <c r="L15" s="46">
         <v>8</v>
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -5861,29 +5898,29 @@
         <v>1.7</v>
       </c>
       <c r="E16" s="38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="11">
         <f t="shared" si="0"/>
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="42">
         <f t="shared" si="1"/>
-        <v>3.125</v>
+        <v>0</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7">
         <f>SUM(I$8:I16)</f>
-        <v>90.625</v>
+        <v>98.4375</v>
       </c>
       <c r="L16" s="45">
         <v>5</v>
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -5906,14 +5943,14 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7">
         <f>SUM(I$8:I17)</f>
-        <v>90.625</v>
+        <v>98.4375</v>
       </c>
       <c r="L17" s="46">
         <v>3</v>
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -5936,14 +5973,14 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7">
         <f>SUM(I$8:I18)</f>
-        <v>92.1875</v>
+        <v>100</v>
       </c>
       <c r="L18" s="45">
         <v>2</v>
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -5951,7 +5988,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="11">
@@ -5961,7 +5998,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="42">
         <f t="shared" si="1"/>
-        <v>7.8125</v>
+        <v>0</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7">
@@ -5973,11 +6010,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="65" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="66"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>64</v>
@@ -5985,7 +6022,7 @@
       <c r="F20" s="22"/>
       <c r="G20" s="23">
         <f>SUM(G8:G19)</f>
-        <v>180.80000000000004</v>
+        <v>214.40000000000003</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="24">
@@ -5995,7 +6032,7 @@
       <c r="J20" s="25"/>
       <c r="K20" s="33">
         <f>FREQUENCY(K8:K19,K21)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L20" s="47">
         <f>SUM(L8:L19)</f>
@@ -6003,61 +6040,61 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="67" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B22" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
+      <c r="C22" s="69"/>
+      <c r="D22" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="60" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="19">
         <f>$G$20</f>
-        <v>180.80000000000004</v>
+        <v>214.40000000000003</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="57" t="s">
+      <c r="N22" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="58">
+      <c r="O22" s="63">
         <f>$L$22/MAX($L$23,1)</f>
-        <v>2.8250000000000006</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="64" t="s">
+        <v>3.3500000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="56"/>
+      <c r="I23" s="61"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>64</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="59"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="N23" s="61"/>
+      <c r="O23" s="64"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -6075,7 +6112,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -6091,14 +6128,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -6112,10 +6149,10 @@
       </c>
       <c r="O27" s="43" t="str">
         <f>IF(K20&lt;&gt;12,INDEX(C8:C19,$K$20+1),"???")</f>
-        <v xml:space="preserve">B </v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+        <v>A–</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D28" s="20" t="s">
         <v>35</v>
       </c>
@@ -6133,14 +6170,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C4:D4"/>
@@ -6153,10 +6182,18 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>depts</formula1>
     </dataValidation>
   </dataValidations>
@@ -6170,7 +6207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6180,78 +6217,78 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.703125" customWidth="1"/>
+    <col min="2" max="2" width="3.703125" customWidth="1"/>
+    <col min="3" max="4" width="8.703125" customWidth="1"/>
+    <col min="5" max="5" width="7.703125" customWidth="1"/>
+    <col min="6" max="6" width="1.703125" customWidth="1"/>
+    <col min="7" max="7" width="7.703125" customWidth="1"/>
+    <col min="8" max="8" width="1.703125" customWidth="1"/>
+    <col min="9" max="9" width="7.703125" customWidth="1"/>
+    <col min="10" max="10" width="1.703125" customWidth="1"/>
+    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.703125" customWidth="1"/>
+    <col min="13" max="13" width="1.703125" customWidth="1"/>
+    <col min="14" max="14" width="3.703125" customWidth="1"/>
+    <col min="15" max="15" width="9.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -6260,59 +6297,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="60" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="60" t="s">
+      <c r="H6" s="50"/>
+      <c r="I6" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="61"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="61"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="50"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62" t="s">
+      <c r="H7" s="52"/>
+      <c r="I7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="62" t="s">
+      <c r="L7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="63"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="52"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -6342,7 +6379,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -6373,7 +6410,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -6403,7 +6440,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -6434,7 +6471,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -6465,7 +6502,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -6496,7 +6533,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -6526,7 +6563,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -6556,7 +6593,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -6586,7 +6623,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -6616,7 +6653,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -6646,7 +6683,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -6676,11 +6713,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="65" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="66"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>0</v>
@@ -6706,24 +6743,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="67" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B22" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
+      <c r="C22" s="69"/>
+      <c r="D22" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="60" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -6733,34 +6770,34 @@
         <v>#VALUE!</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="57" t="s">
+      <c r="N22" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="58" t="e">
+      <c r="O22" s="63" t="e">
         <f>$L$22/MAX($L$23,1)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="64" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="56"/>
+      <c r="I23" s="61"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="59"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="N23" s="61"/>
+      <c r="O23" s="64"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -6778,7 +6815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -6794,14 +6831,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -6818,7 +6855,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D28" s="20" t="s">
         <v>59</v>
       </c>
@@ -6836,6 +6873,10 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G6:H6"/>
@@ -6852,14 +6893,10 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>depts</formula1>
     </dataValidation>
   </dataValidations>
@@ -6873,7 +6910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6883,78 +6920,78 @@
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="1.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.703125" customWidth="1"/>
+    <col min="2" max="2" width="3.703125" customWidth="1"/>
+    <col min="3" max="4" width="8.703125" customWidth="1"/>
+    <col min="5" max="5" width="7.703125" customWidth="1"/>
+    <col min="6" max="6" width="1.703125" customWidth="1"/>
+    <col min="7" max="7" width="7.703125" customWidth="1"/>
+    <col min="8" max="8" width="1.703125" customWidth="1"/>
+    <col min="9" max="9" width="7.703125" customWidth="1"/>
+    <col min="10" max="10" width="1.703125" customWidth="1"/>
+    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.703125" customWidth="1"/>
+    <col min="13" max="13" width="1.703125" customWidth="1"/>
+    <col min="14" max="14" width="3.703125" customWidth="1"/>
+    <col min="15" max="15" width="9.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -6963,59 +7000,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="60" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="60" t="s">
+      <c r="H6" s="50"/>
+      <c r="I6" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="61"/>
+      <c r="J6" s="50"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="61"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="50"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="62" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62" t="s">
+      <c r="H7" s="52"/>
+      <c r="I7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="52"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="62" t="s">
+      <c r="L7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="63"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="52"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -7043,7 +7080,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -7072,7 +7109,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -7100,7 +7137,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -7129,7 +7166,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -7158,7 +7195,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -7187,7 +7224,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -7215,7 +7252,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -7243,7 +7280,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -7271,7 +7308,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -7299,7 +7336,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -7327,7 +7364,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -7355,11 +7392,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="65" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="66"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>0</v>
@@ -7385,24 +7422,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="67" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B22" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
+      <c r="C22" s="69"/>
+      <c r="D22" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="55" t="s">
+      <c r="I22" s="60" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -7412,34 +7449,34 @@
         <v>0</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="57" t="s">
+      <c r="N22" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="58">
+      <c r="O22" s="63">
         <f>$L$22/MAX($L$23,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="64" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="56"/>
+      <c r="I23" s="61"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="59"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="N23" s="61"/>
+      <c r="O23" s="64"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -7457,7 +7494,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -7473,14 +7510,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -7497,7 +7534,7 @@
         <v>???</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
       <c r="D28" s="20" t="s">
         <v>60</v>
       </c>
@@ -7515,14 +7552,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C4:D4"/>
@@ -7535,10 +7564,18 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:G3" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>depts</formula1>
     </dataValidation>
   </dataValidations>
@@ -7552,18 +7589,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -7583,7 +7620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -7603,7 +7640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -7623,7 +7660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -7643,7 +7680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -7663,7 +7700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E6" t="s">
         <v>7</v>
       </c>
@@ -7680,7 +7717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E7" t="s">
         <v>23</v>
       </c>
@@ -7697,7 +7734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>8</v>
       </c>
@@ -7714,7 +7751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E9" t="s">
         <v>9</v>
       </c>
@@ -7731,7 +7768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E10" t="s">
         <v>24</v>
       </c>
@@ -7748,7 +7785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E11" t="s">
         <v>10</v>
       </c>
@@ -7765,7 +7802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E12" t="s">
         <v>16</v>
       </c>
@@ -7782,7 +7819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E13" t="s">
         <v>11</v>
       </c>
@@ -7799,7 +7836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E15" t="s">
         <v>17</v>
       </c>
@@ -7816,7 +7853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E16" t="s">
         <v>49</v>
       </c>
@@ -7833,7 +7870,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:9" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
         <v>50</v>
       </c>
@@ -7850,7 +7887,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:9" x14ac:dyDescent="0.4">
       <c r="F18">
         <v>2.6</v>
       </c>

</xml_diff>

<commit_message>
added more detailed error msg
</commit_message>
<xml_diff>
--- a/Example/Distribution Files/F1997/MEC E 260 - 502 (77588) Ayranci/MecE260_UNDERGRAD Grade Dist Form.xlsx
+++ b/Example/Distribution Files/F1997/MEC E 260 - 502 (77588) Ayranci/MecE260_UNDERGRAD Grade Dist Form.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\Processing_Folders\Example\Distribution Files\F1997\MEC E 260 - 502 (77588) Ayranci\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jas98\Work\Processing_Folders\Example\Distribution Files\F1997\MEC E 260 - 502 (77588) Ayranci\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B7D2BB-7D2B-4556-A957-BC4B63C345C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D573D0-4521-4387-864E-998B843433CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1522,10 +1522,10 @@
     <t>A1</t>
   </si>
   <si>
-    <t>Aryanci</t>
+    <t>MECE 260</t>
   </si>
   <si>
-    <t>MECE 260</t>
+    <t>lllllll</t>
   </si>
 </sst>
 </file>
@@ -1913,21 +1913,6 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1966,6 +1951,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1977,6 +1974,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4753,29 +4753,29 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -4799,82 +4799,82 @@
       <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.703125" customWidth="1"/>
-    <col min="2" max="2" width="3.703125" customWidth="1"/>
-    <col min="3" max="4" width="8.703125" customWidth="1"/>
-    <col min="5" max="5" width="7.703125" customWidth="1"/>
-    <col min="6" max="6" width="1.703125" customWidth="1"/>
-    <col min="7" max="7" width="7.703125" customWidth="1"/>
-    <col min="8" max="8" width="1.703125" customWidth="1"/>
-    <col min="9" max="9" width="7.703125" customWidth="1"/>
-    <col min="10" max="10" width="1.703125" customWidth="1"/>
-    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.703125" customWidth="1"/>
-    <col min="13" max="13" width="1.703125" customWidth="1"/>
-    <col min="14" max="14" width="3.703125" customWidth="1"/>
-    <col min="15" max="15" width="9.703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="59"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -4883,59 +4883,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="50"/>
-      <c r="G6" s="49" t="s">
+      <c r="F6" s="61"/>
+      <c r="G6" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="49" t="s">
+      <c r="H6" s="61"/>
+      <c r="I6" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="50"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="50"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="51" t="s">
+      <c r="H7" s="63"/>
+      <c r="I7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="52"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="52"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -4996,7 +4996,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -5057,7 +5057,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -5088,7 +5088,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -5119,7 +5119,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -5179,7 +5179,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -5269,7 +5269,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -5299,11 +5299,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="66" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="67"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>0</v>
@@ -5329,24 +5329,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B22" s="68" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="53" t="s">
+      <c r="C22" s="68"/>
+      <c r="D22" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="60" t="s">
+      <c r="I22" s="55" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -5356,34 +5356,34 @@
         <v>#VALUE!</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="62" t="s">
+      <c r="N22" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="63" t="e">
+      <c r="O22" s="58" t="e">
         <f>$L$22/MAX($L$23,1)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="65" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="61"/>
+      <c r="I23" s="56"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="64"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="N23" s="56"/>
+      <c r="O23" s="59"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -5417,14 +5417,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -5441,7 +5441,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D28" s="20" t="s">
         <v>58</v>
       </c>
@@ -5459,10 +5459,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G6:H6"/>
@@ -5479,6 +5475,10 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -5503,89 +5503,89 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.703125" customWidth="1"/>
-    <col min="2" max="2" width="3.703125" customWidth="1"/>
-    <col min="3" max="4" width="8.703125" customWidth="1"/>
-    <col min="5" max="5" width="7.703125" customWidth="1"/>
-    <col min="6" max="6" width="1.703125" customWidth="1"/>
-    <col min="7" max="7" width="7.703125" customWidth="1"/>
-    <col min="8" max="8" width="1.703125" customWidth="1"/>
-    <col min="9" max="9" width="7.703125" customWidth="1"/>
-    <col min="10" max="10" width="1.703125" customWidth="1"/>
-    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.703125" customWidth="1"/>
-    <col min="13" max="13" width="1.703125" customWidth="1"/>
-    <col min="14" max="14" width="3.703125" customWidth="1"/>
-    <col min="15" max="15" width="9.703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="L3" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="57"/>
+      <c r="C4" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="52"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="59"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -5594,59 +5594,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="50"/>
-      <c r="G6" s="49" t="s">
+      <c r="F6" s="61"/>
+      <c r="G6" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="49" t="s">
+      <c r="H6" s="61"/>
+      <c r="I6" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="50"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="50"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="51" t="s">
+      <c r="H7" s="63"/>
+      <c r="I7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="52"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="52"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -5707,7 +5707,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -5768,7 +5768,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -5799,7 +5799,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -5830,7 +5830,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -5860,7 +5860,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -5920,7 +5920,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -6010,11 +6010,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="66" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="67"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>64</v>
@@ -6040,24 +6040,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B22" s="68" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="53" t="s">
+      <c r="C22" s="68"/>
+      <c r="D22" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="60" t="s">
+      <c r="I22" s="55" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -6067,34 +6067,34 @@
         <v>214.40000000000003</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="62" t="s">
+      <c r="N22" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="63">
+      <c r="O22" s="58">
         <f>$L$22/MAX($L$23,1)</f>
         <v>3.3500000000000005</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="65" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="61"/>
+      <c r="I23" s="56"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>64</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="64"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="N23" s="56"/>
+      <c r="O23" s="59"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -6128,14 +6128,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -6152,7 +6152,7 @@
         <v>A–</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D28" s="20" t="s">
         <v>35</v>
       </c>
@@ -6170,6 +6170,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C4:D4"/>
@@ -6182,14 +6190,6 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -6217,78 +6217,78 @@
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.703125" customWidth="1"/>
-    <col min="2" max="2" width="3.703125" customWidth="1"/>
-    <col min="3" max="4" width="8.703125" customWidth="1"/>
-    <col min="5" max="5" width="7.703125" customWidth="1"/>
-    <col min="6" max="6" width="1.703125" customWidth="1"/>
-    <col min="7" max="7" width="7.703125" customWidth="1"/>
-    <col min="8" max="8" width="1.703125" customWidth="1"/>
-    <col min="9" max="9" width="7.703125" customWidth="1"/>
-    <col min="10" max="10" width="1.703125" customWidth="1"/>
-    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.703125" customWidth="1"/>
-    <col min="13" max="13" width="1.703125" customWidth="1"/>
-    <col min="14" max="14" width="3.703125" customWidth="1"/>
-    <col min="15" max="15" width="9.703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -6297,59 +6297,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="50"/>
-      <c r="G6" s="49" t="s">
+      <c r="F6" s="61"/>
+      <c r="G6" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="49" t="s">
+      <c r="H6" s="61"/>
+      <c r="I6" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="50"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="50"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="51" t="s">
+      <c r="H7" s="63"/>
+      <c r="I7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="52"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="52"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -6410,7 +6410,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -6440,7 +6440,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -6471,7 +6471,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -6502,7 +6502,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -6533,7 +6533,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -6593,7 +6593,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -6623,7 +6623,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -6653,7 +6653,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -6683,7 +6683,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -6713,11 +6713,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="66" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="67"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>0</v>
@@ -6743,24 +6743,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B22" s="68" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="53" t="s">
+      <c r="C22" s="68"/>
+      <c r="D22" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="60" t="s">
+      <c r="I22" s="55" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -6770,34 +6770,34 @@
         <v>#VALUE!</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="62" t="s">
+      <c r="N22" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="63" t="e">
+      <c r="O22" s="58" t="e">
         <f>$L$22/MAX($L$23,1)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="65" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="61"/>
+      <c r="I23" s="56"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="64"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="N23" s="56"/>
+      <c r="O23" s="59"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -6831,14 +6831,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -6855,7 +6855,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D28" s="20" t="s">
         <v>59</v>
       </c>
@@ -6873,10 +6873,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G6:H6"/>
@@ -6893,6 +6889,10 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -6920,78 +6920,78 @@
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.703125" customWidth="1"/>
-    <col min="2" max="2" width="3.703125" customWidth="1"/>
-    <col min="3" max="4" width="8.703125" customWidth="1"/>
-    <col min="5" max="5" width="7.703125" customWidth="1"/>
-    <col min="6" max="6" width="1.703125" customWidth="1"/>
-    <col min="7" max="7" width="7.703125" customWidth="1"/>
-    <col min="8" max="8" width="1.703125" customWidth="1"/>
-    <col min="9" max="9" width="7.703125" customWidth="1"/>
-    <col min="10" max="10" width="1.703125" customWidth="1"/>
-    <col min="11" max="11" width="9.5859375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.703125" customWidth="1"/>
-    <col min="13" max="13" width="1.703125" customWidth="1"/>
-    <col min="14" max="14" width="3.703125" customWidth="1"/>
-    <col min="15" max="15" width="9.703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="1.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.35" x14ac:dyDescent="0.5">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
@@ -7000,59 +7000,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="50"/>
-      <c r="G6" s="49" t="s">
+      <c r="F6" s="61"/>
+      <c r="G6" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="49" t="s">
+      <c r="H6" s="61"/>
+      <c r="I6" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="50"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="50"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="51" t="s">
+      <c r="H7" s="63"/>
+      <c r="I7" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="52"/>
+      <c r="J7" s="63"/>
       <c r="K7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="52"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
@@ -7109,7 +7109,7 @@
       <c r="M9" s="15"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
@@ -7166,7 +7166,7 @@
       <c r="M11" s="15"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>7</v>
       </c>
@@ -7195,7 +7195,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
@@ -7224,7 +7224,7 @@
       <c r="M13" s="15"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
@@ -7252,7 +7252,7 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
@@ -7280,7 +7280,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
@@ -7308,7 +7308,7 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="9" t="s">
         <v>10</v>
       </c>
@@ -7336,7 +7336,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
@@ -7364,7 +7364,7 @@
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
@@ -7392,11 +7392,11 @@
       </c>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="66" t="s">
+    <row r="20" spans="2:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="67"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="37">
         <f>SUM(E8:E19)</f>
         <v>0</v>
@@ -7422,24 +7422,24 @@
       </c>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K21">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B22" s="68" t="s">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="53" t="s">
+      <c r="C22" s="68"/>
+      <c r="D22" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="60" t="s">
+      <c r="I22" s="55" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4"/>
@@ -7449,34 +7449,34 @@
         <v>0</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="62" t="s">
+      <c r="N22" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="O22" s="63">
+      <c r="O22" s="58">
         <f>$L$22/MAX($L$23,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="65" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="61"/>
+      <c r="I23" s="56"/>
       <c r="L23" s="1">
         <f>$E$20</f>
         <v>0</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="64"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="N23" s="56"/>
+      <c r="O23" s="59"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>34</v>
@@ -7510,14 +7510,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -7534,7 +7534,7 @@
         <v>???</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D28" s="20" t="s">
         <v>60</v>
       </c>
@@ -7552,6 +7552,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C4:D4"/>
@@ -7564,14 +7572,6 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -7595,12 +7595,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>7</v>
       </c>
@@ -7717,7 +7717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>23</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>8</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>9</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>24</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>10</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>16</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>11</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>17</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>49</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>50</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>2.6</v>
       </c>

</xml_diff>